<commit_message>
Added Missiles with Targeting
</commit_message>
<xml_diff>
--- a/Fighter Settings.xlsx
+++ b/Fighter Settings.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ModProject 4.27\Content\GlutenFighters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fc1a16f306d1bae/Unreal/ModProject/Content/GlutenFighters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{873F28C5-D956-4CE6-82FC-51B6E7FF8776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{873F28C5-D956-4CE6-82FC-51B6E7FF8776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDFFB890-8991-44F5-95D8-E4A0127D7BA5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BDDC6CC-D353-44B8-BD89-5FFC240C0369}"/>
+    <workbookView xWindow="-98" yWindow="13403" windowWidth="21795" windowHeight="12975" xr2:uid="{0BDDC6CC-D353-44B8-BD89-5FFC240C0369}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Fighter Name</t>
   </si>
@@ -103,13 +102,37 @@
   </si>
   <si>
     <t>DPS</t>
+  </si>
+  <si>
+    <t># of Bolts Firing at a Time</t>
+  </si>
+  <si>
+    <t>TIE Fighter</t>
+  </si>
+  <si>
+    <t>TIE Interceptor</t>
+  </si>
+  <si>
+    <t>TIE Bomber</t>
+  </si>
+  <si>
+    <t>Troop Transport</t>
+  </si>
+  <si>
+    <t>A-Wing</t>
+  </si>
+  <si>
+    <t>X-Wing</t>
+  </si>
+  <si>
+    <t>Y-Wing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +147,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +165,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,9 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,26 +539,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68835544-F02A-48E3-8982-3FA93D4E0B31}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,274 +584,553 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>5000</v>
-      </c>
-      <c r="D2">
-        <v>45</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
-      </c>
-      <c r="F2">
-        <v>45</v>
-      </c>
-      <c r="G2">
-        <v>500</v>
-      </c>
-      <c r="H2">
-        <v>75</v>
-      </c>
-      <c r="I2">
+      <c r="C2" s="2">
+        <v>5250</v>
+      </c>
+      <c r="D2" s="2">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>250</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K2" s="4">
+        <f>ROUND((H2/J2)*I2,0)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4750</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>750</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K16" si="0">ROUND((H3/J3)*I3,0)</f>
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5250</v>
+      </c>
+      <c r="D4" s="2">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>200</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
         <v>0.1</v>
       </c>
-      <c r="J2">
-        <f>(H2/I2)</f>
+      <c r="K4" s="4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5250</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2">
+        <v>50</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1500</v>
+      </c>
+      <c r="H5" s="2">
+        <v>700</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5250</v>
+      </c>
+      <c r="D6" s="2">
+        <v>50</v>
+      </c>
+      <c r="E6" s="2">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="H6" s="2">
+        <v>400</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5250</v>
+      </c>
+      <c r="D7" s="2">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>200</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4750</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H8" s="2">
         <v>750</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="0"/>
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>4000</v>
-      </c>
-      <c r="D3">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>35</v>
-      </c>
-      <c r="F3">
-        <v>35</v>
-      </c>
-      <c r="G3">
+      <c r="C9" s="2">
+        <v>4750</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2">
+        <v>45</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>750</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="0"/>
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5250</v>
+      </c>
+      <c r="D10" s="3">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3">
+        <v>50</v>
+      </c>
+      <c r="F10" s="3">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1500</v>
+      </c>
+      <c r="H10" s="3">
+        <v>250</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5250</v>
+      </c>
+      <c r="D11" s="3">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3">
         <v>1000</v>
       </c>
-      <c r="H3">
-        <v>400</v>
-      </c>
-      <c r="I3">
-        <v>0.35</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J9" si="0">(H3/I3)</f>
-        <v>1142.8571428571429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="H11" s="3">
+        <v>150</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4750</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3">
+        <v>45</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3000</v>
+      </c>
+      <c r="H12" s="3">
+        <v>750</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4750</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45</v>
+      </c>
+      <c r="E13" s="3">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3">
+        <v>45</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3000</v>
+      </c>
+      <c r="H13" s="3">
+        <v>750</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
-        <v>5000</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>45</v>
-      </c>
-      <c r="G4">
-        <v>500</v>
-      </c>
-      <c r="H4">
-        <v>75</v>
-      </c>
-      <c r="I4">
+      <c r="C14" s="3">
+        <v>5250</v>
+      </c>
+      <c r="D14" s="3">
+        <v>55</v>
+      </c>
+      <c r="E14" s="3">
+        <v>55</v>
+      </c>
+      <c r="F14" s="3">
+        <v>55</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="3">
+        <v>250</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
         <v>0.1</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="K14" s="4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>4500</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5">
-        <v>40</v>
-      </c>
-      <c r="G5">
-        <v>750</v>
-      </c>
-      <c r="H5">
-        <v>200</v>
-      </c>
-      <c r="I5">
-        <v>0.2</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>4500</v>
-      </c>
-      <c r="D6">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
-      </c>
-      <c r="G6">
-        <v>750</v>
-      </c>
-      <c r="H6">
-        <v>200</v>
-      </c>
-      <c r="I6">
-        <v>0.2</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>5000</v>
-      </c>
-      <c r="D7">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>45</v>
-      </c>
-      <c r="F7">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>500</v>
-      </c>
-      <c r="H7">
-        <v>75</v>
-      </c>
-      <c r="I7">
-        <v>0.1</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C15" s="3">
+        <v>5250</v>
+      </c>
+      <c r="D15" s="3">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3">
+        <v>50</v>
+      </c>
+      <c r="F15" s="3">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1500</v>
+      </c>
+      <c r="H15" s="3">
+        <v>300</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>4000</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>35</v>
-      </c>
-      <c r="F8">
-        <v>35</v>
-      </c>
-      <c r="G8">
-        <v>1000</v>
-      </c>
-      <c r="H8">
-        <v>400</v>
-      </c>
-      <c r="I8">
-        <v>0.35</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1142.8571428571429</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>4000</v>
-      </c>
-      <c r="D9">
-        <v>35</v>
-      </c>
-      <c r="E9">
-        <v>35</v>
-      </c>
-      <c r="F9">
-        <v>35</v>
-      </c>
-      <c r="G9">
-        <v>1000</v>
-      </c>
-      <c r="H9">
-        <v>400</v>
-      </c>
-      <c r="I9">
-        <v>0.35</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>1142.8571428571429</v>
+      <c r="C16" s="3">
+        <v>4750</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45</v>
+      </c>
+      <c r="F16" s="3">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3000</v>
+      </c>
+      <c r="H16" s="3">
+        <v>375</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>